<commit_message>
fixed #854 FlixelGames-854 強化時のメッセージ表示
</commit_message>
<xml_diff>
--- a/OneWayRPG3/docs/message.xlsx
+++ b/OneWayRPG3/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>id</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>アイテムがないので自動攻撃</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;を強化した</t>
+  </si>
+  <si>
+    <t>最大HPが&lt;val1&gt;上昇した</t>
   </si>
   <si>
     <t>攻撃力</t>
@@ -1565,7 +1571,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1601,7 +1607,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" si="0" ref="A3:A67">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A69">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2377,6 +2383,30 @@
       </c>
       <c r="C67" t="s" s="4">
         <v>10</v>
+      </c>
+    </row>
+    <row r="68" ht="20" customHeight="1">
+      <c r="A68" s="5">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B68" t="s" s="4">
+        <v>76</v>
+      </c>
+      <c r="C68" t="s" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" ht="20" customHeight="1">
+      <c r="A69" s="5">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B69" t="s" s="4">
+        <v>77</v>
+      </c>
+      <c r="C69" t="s" s="4">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2426,7 +2456,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -2435,7 +2465,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -2444,7 +2474,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -2453,7 +2483,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -2462,7 +2492,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -2471,7 +2501,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -2480,7 +2510,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -2489,7 +2519,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -2498,7 +2528,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -2507,7 +2537,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -2516,7 +2546,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -2525,7 +2555,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -2534,7 +2564,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -2543,7 +2573,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -2552,7 +2582,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -2561,7 +2591,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -2570,7 +2600,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -2579,7 +2609,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -2588,7 +2618,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
@@ -2597,7 +2627,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
@@ -2606,7 +2636,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
@@ -2615,7 +2645,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
@@ -2624,7 +2654,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
@@ -2633,7 +2663,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
@@ -2642,7 +2672,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
@@ -2651,7 +2681,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
@@ -2660,7 +2690,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
@@ -2669,7 +2699,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
@@ -2678,7 +2708,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
@@ -2687,7 +2717,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
@@ -2696,7 +2726,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -2714,7 +2744,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -2723,7 +2753,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
@@ -2732,7 +2762,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
@@ -2741,7 +2771,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>